<commit_message>
Revised ESST1A input file.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_esst1a.xlsx
+++ b/andes/cases/ieee14/ieee14_esst1a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1919BF6D-6256-6540-9116-617310660B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF28F96F-713F-BF4B-9616-2AACCF4B4C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="170">
   <si>
     <t>idx</t>
   </si>
@@ -1890,7 +1890,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1937,8 +1937,8 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>169</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>